<commit_message>
just incorporated Taras's edits
</commit_message>
<xml_diff>
--- a/Manuscripts/JournalPaper/mint_defense or receptors.xlsx
+++ b/Manuscripts/JournalPaper/mint_defense or receptors.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://emailwsu-my.sharepoint.com/personal/sudha_gcupadhaya_wsu_edu/Documents/Desktop/New folder/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidlinnardwheeler/Desktop/Desktop - David’s MacBook Pro/Research/RNA-seq/Manuscripts/JournalPaper/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="30" documentId="8_{FE88F0E1-804C-4CCE-91C6-B2E968D8B878}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EBDCF176-6C07-4FEE-9252-3B1CFA89DFA1}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58AE7C13-F7FF-CB41-A4BB-4E06293DD5FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="17115" windowHeight="10876" xr2:uid="{0F00692D-60A1-41F1-A309-1ACF0F69DFC1}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="17120" windowHeight="10880" xr2:uid="{0F00692D-60A1-41F1-A309-1ACF0F69DFC1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -637,20 +637,21 @@
   <dimension ref="A1:L20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N9" sqref="N9"/>
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="8" max="8" width="18.86328125" customWidth="1"/>
+    <col min="7" max="7" width="15.33203125" customWidth="1"/>
+    <col min="8" max="8" width="18.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="L1" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -688,7 +689,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -726,7 +727,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -764,7 +765,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -802,7 +803,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -840,7 +841,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>0</v>
       </c>
@@ -878,7 +879,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>0</v>
       </c>
@@ -916,7 +917,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>0</v>
       </c>
@@ -954,7 +955,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>0</v>
       </c>
@@ -989,7 +990,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>0</v>
       </c>
@@ -1024,7 +1025,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>0</v>
       </c>
@@ -1062,7 +1063,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>0</v>
       </c>
@@ -1097,7 +1098,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>0</v>
       </c>
@@ -1132,7 +1133,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>0</v>
       </c>
@@ -1167,7 +1168,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>0</v>
       </c>
@@ -1202,7 +1203,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>0</v>
       </c>
@@ -1237,7 +1238,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>0</v>
       </c>
@@ -1275,7 +1276,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>0</v>
       </c>
@@ -1313,7 +1314,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>0</v>
       </c>
@@ -1366,6 +1367,12 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A405498542C8C3489A26ED31B6FB6BC7" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e55056d16f9a16ddf1f9ebe4ca964fa2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="801f6cec-90ea-4220-916e-6af857acad63" xmlns:ns4="75a8b541-bace-45e5-b228-00a14a4a2df8" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="344f4c16c82d69bd5c0449d16e23717b" ns3:_="" ns4:_="">
     <xsd:import namespace="801f6cec-90ea-4220-916e-6af857acad63"/>
@@ -1594,12 +1601,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C485C286-33D2-4DAC-8401-F65FFF337E84}">
   <ds:schemaRefs>
@@ -1609,6 +1610,23 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{37289CCC-73ED-4B61-AA0F-C5C332EB352A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="75a8b541-bace-45e5-b228-00a14a4a2df8"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="801f6cec-90ea-4220-916e-6af857acad63"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{391FE937-2BD7-4586-8000-29EB59C568D7}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1625,21 +1643,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{37289CCC-73ED-4B61-AA0F-C5C332EB352A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="75a8b541-bace-45e5-b228-00a14a4a2df8"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="801f6cec-90ea-4220-916e-6af857acad63"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>